<commit_message>
Add second factor to 0-var baseline-invariant test
Updates both test and fixture, with a sort disabled in the test to demo that the test can fail.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/stata_results/tooyoung_baseline_invariant/tooyoung_baseline_invariant.xlsx
+++ b/tests/testthat/fixtures/stata_results/tooyoung_baseline_invariant/tooyoung_baseline_invariant.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="30" uniqueCount="16">
   <si>
     <t>ln_real_wage</t>
   </si>
@@ -51,6 +51,12 @@
     <t>advanced_degree</t>
   </si>
   <si>
+    <t>foreign_born</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
     <t>Intercept</t>
   </si>
   <si>
@@ -65,7 +71,127 @@
     <numFmt numFmtId="166" formatCode="0.######"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="124">
+  <fonts count="154">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -571,7 +697,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="124">
+  <borders count="154">
     <border>
       <left/>
       <right/>
@@ -1409,6 +1535,216 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="thin"/>
       <diagonal style="none"/>
     </border>
@@ -1444,7 +1780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1918,23 +2254,143 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="0" borderId="119" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="120" fillId="0" borderId="120" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="121" fillId="0" borderId="121" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="122" fillId="0" borderId="122" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="123" fillId="0" borderId="123" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="119" fillId="0" borderId="119" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="120" fillId="0" borderId="120" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="121" fillId="0" borderId="121" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="122" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="123" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="124" fillId="0" borderId="124" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="125" fillId="0" borderId="125" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="126" fillId="0" borderId="126" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="127" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="128" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="129" fillId="0" borderId="129" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="130" fillId="0" borderId="130" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="131" fillId="0" borderId="131" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="132" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="133" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="134" fillId="0" borderId="134" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="135" fillId="0" borderId="135" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="136" fillId="0" borderId="136" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="137" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="0" borderId="138" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="139" fillId="0" borderId="139" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="140" fillId="0" borderId="140" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="141" fillId="0" borderId="141" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="142" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="143" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="144" fillId="0" borderId="144" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="145" fillId="0" borderId="145" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="146" fillId="0" borderId="146" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="147" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="148" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="149" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="150" fillId="0" borderId="150" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="151" fillId="0" borderId="151" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="152" fillId="0" borderId="152" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="153" fillId="0" borderId="153" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1947,7 +2403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1964,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="11">
-        <v>2.6254132011217868</v>
+        <v>2.6254132011217872</v>
       </c>
     </row>
     <row r="3">
@@ -1980,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21">
-        <v>0.52629077772971122</v>
+        <v>0.52629077772971167</v>
       </c>
     </row>
     <row r="5">
@@ -1988,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26">
-        <v>-0.024974598191149333</v>
+        <v>-0.14134725004044157</v>
       </c>
     </row>
     <row r="6">
@@ -1996,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="31">
-        <v>0.33696917789699388</v>
+        <v>0.36006751649960878</v>
       </c>
     </row>
     <row r="7">
@@ -2004,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="36">
-        <v>0.21429619802386668</v>
+        <v>0.30757051127054447</v>
       </c>
     </row>
     <row r="8">
@@ -2012,7 +2468,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="41">
-        <v>-0.023876935495955605</v>
+        <v>-0.016966524969175206</v>
       </c>
     </row>
     <row r="9">
@@ -2020,7 +2476,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46">
-        <v>0.011675139576151032</v>
+        <v>0.0082961461771727373</v>
       </c>
     </row>
     <row r="10">
@@ -2028,7 +2484,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="51">
-        <v>0.0049006758714708037</v>
+        <v>0.0034823329632576927</v>
       </c>
     </row>
     <row r="11">
@@ -2036,7 +2492,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="56">
-        <v>-0.01997967855291943</v>
+        <v>-0.014197203619435208</v>
       </c>
     </row>
     <row r="12">
@@ -2044,44 +2500,44 @@
         <v>11</v>
       </c>
       <c r="B12" s="61">
-        <v>0.0023062004101039079</v>
+        <v>0.0016387449238859729</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="63" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B13" s="66">
-        <v>-0.33261387726511932</v>
+        <v>-0.061800372758073749</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="68" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B14" s="71">
-        <v>0</v>
+        <v>-0.061800372758073749</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="73" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" s="76">
-        <v>0</v>
+        <v>-0.31308678434359039</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="81">
-        <v>-0.0092367579075557892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="83" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="86">
         <v>0</v>
@@ -2089,57 +2545,105 @@
     </row>
     <row r="18">
       <c r="A18" s="88" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="91">
-        <v>0.67881981306966921</v>
+        <v>-0.020999136776596788</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="93" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B19" s="96">
-        <v>0.21938253742432909</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="98" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20" s="101">
-        <v>-0.037949285142984832</v>
+        <v>0.019703207601276584</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="103" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B21" s="106">
-        <v>0.012209953833815797</v>
+        <v>-0.10836764180702121</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="108" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B22" s="111">
-        <v>-0.0042482485322653217</v>
+        <v>0.78281787182554075</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="116">
+        <v>0.2065030291221813</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="118" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="121">
+        <v>-0.036428013282573529</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="126">
+        <v>0.013373256452303629</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="131">
+        <v>-0.0096581022132280273</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="116">
-        <v>0.024901240440972236</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="119" t="s">
+      <c r="B27" s="136">
+        <v>0.025307092605966166</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="141">
+        <v>0.054236624292947413</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="123">
+      <c r="B29" s="146">
+        <v>0.054236624292947413</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="149" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="153">
         <v>666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Swap viewpoint groups to force non-zero estimates
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/stata_results/tooyoung_baseline_invariant/tooyoung_baseline_invariant.xlsx
+++ b/tests/testthat/fixtures/stata_results/tooyoung_baseline_invariant/tooyoung_baseline_invariant.xlsx
@@ -15,7 +15,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="30" uniqueCount="16">
   <si>
-    <t>ln_real_wage</t>
+    <t>unwage</t>
   </si>
   <si>
     <t>group_1</t>
@@ -2420,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="11">
-        <v>2.6254132011217872</v>
+        <v>-2.0991224233920756</v>
       </c>
     </row>
     <row r="3">
@@ -2428,7 +2428,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="16">
-        <v>2.0991224233920756</v>
+        <v>-2.6254132011217872</v>
       </c>
     </row>
     <row r="4">
@@ -2444,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26">
-        <v>-0.14134725004044157</v>
+        <v>0.16622326123010289</v>
       </c>
     </row>
     <row r="6">
@@ -2452,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="31">
-        <v>0.36006751649960878</v>
+        <v>0.66763802777015324</v>
       </c>
     </row>
     <row r="7">
@@ -2460,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="36">
-        <v>0.30757051127054447</v>
+        <v>-0.30757051127054469</v>
       </c>
     </row>
     <row r="8">
@@ -2468,7 +2468,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="41">
-        <v>-0.016966524969175206</v>
+        <v>0.18953650415300607</v>
       </c>
     </row>
     <row r="9">
@@ -2476,7 +2476,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46">
-        <v>0.0082961461771727373</v>
+        <v>-0.02813186710540079</v>
       </c>
     </row>
     <row r="10">
@@ -2484,7 +2484,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="51">
-        <v>0.0034823329632576927</v>
+        <v>0.016855589415561322</v>
       </c>
     </row>
     <row r="11">
@@ -2492,7 +2492,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="56">
-        <v>-0.014197203619435208</v>
+        <v>-0.023855305832663234</v>
       </c>
     </row>
     <row r="12">
@@ -2500,7 +2500,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="61">
-        <v>0.0016387449238859729</v>
+        <v>0.026945837529852138</v>
       </c>
     </row>
     <row r="13">
@@ -2508,7 +2508,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="66">
-        <v>-0.061800372758073749</v>
+        <v>-0.0075637484651263362</v>
       </c>
     </row>
     <row r="14">
@@ -2516,7 +2516,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="71">
-        <v>-0.061800372758073749</v>
+        <v>-0.0075637484651263362</v>
       </c>
     </row>
     <row r="15">
@@ -2524,7 +2524,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="76">
-        <v>-0.31308678434359039</v>
+        <v>-0.10658375522140909</v>
       </c>
     </row>
     <row r="16">
@@ -2532,7 +2532,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="81">
-        <v>0</v>
+        <v>-0.036428013282573529</v>
       </c>
     </row>
     <row r="17">
@@ -2540,7 +2540,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="86">
-        <v>0</v>
+        <v>0.013373256452303629</v>
       </c>
     </row>
     <row r="18">
@@ -2548,7 +2548,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="91">
-        <v>-0.020999136776596788</v>
+        <v>-0.030657238989824816</v>
       </c>
     </row>
     <row r="19">
@@ -2556,7 +2556,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="96">
-        <v>0</v>
+        <v>0.025307092605966166</v>
       </c>
     </row>
     <row r="20">
@@ -2564,7 +2564,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="101">
-        <v>0.019703207601276584</v>
+        <v>0.073939831894223998</v>
       </c>
     </row>
     <row r="21">
@@ -2572,7 +2572,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="106">
-        <v>-0.10836764180702121</v>
+        <v>-0.054131017514073801</v>
       </c>
     </row>
     <row r="22">
@@ -2588,7 +2588,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="116">
-        <v>0.2065030291221813</v>
+        <v>-0.2065030291221813</v>
       </c>
     </row>
     <row r="24">
@@ -2596,7 +2596,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="121">
-        <v>-0.036428013282573529</v>
+        <v>0.036428013282573529</v>
       </c>
     </row>
     <row r="25">
@@ -2604,7 +2604,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="126">
-        <v>0.013373256452303629</v>
+        <v>-0.013373256452303629</v>
       </c>
     </row>
     <row r="26">
@@ -2612,7 +2612,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="131">
-        <v>-0.0096581022132280273</v>
+        <v>0.0096581022132280273</v>
       </c>
     </row>
     <row r="27">
@@ -2620,7 +2620,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="136">
-        <v>0.025307092605966166</v>
+        <v>-0.025307092605966166</v>
       </c>
     </row>
     <row r="28">
@@ -2628,7 +2628,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="141">
-        <v>0.054236624292947413</v>
+        <v>-0.054236624292947413</v>
       </c>
     </row>
     <row r="29">
@@ -2636,7 +2636,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="146">
-        <v>0.054236624292947413</v>
+        <v>-0.054236624292947413</v>
       </c>
     </row>
     <row r="30">

</xml_diff>